<commit_message>
BTTuan11, PTPMHDT_ BT Winform
</commit_message>
<xml_diff>
--- a/tuần 10/1150080069_TranDuongYenNhi_bth9_QLDAxlsx.xlsx
+++ b/tuần 10/1150080069_TranDuongYenNhi_bth9_QLDAxlsx.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QLDA\PP-PT-PMHDT\tuần 10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB1C815-AFD7-4BB4-9FD9-9E94AAF13F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1754267-A608-48FD-BE71-5EAD017ECB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2240" yWindow="2240" windowWidth="19200" windowHeight="11170" xr2:uid="{1403AE77-F9C8-4D41-AC0B-ADAE059B06CE}"/>
   </bookViews>
   <sheets>
     <sheet name="WSM" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>WIEGHT</t>
   </si>
@@ -83,6 +84,30 @@
   </si>
   <si>
     <t>TỔNG ĐIỂM CÓ TRỌNG SỐ</t>
+  </si>
+  <si>
+    <t>Giao diện thân thiện, dễ dùng</t>
+  </si>
+  <si>
+    <t>Tốc độ xử lý &amp; truy cập</t>
+  </si>
+  <si>
+    <t>Tính ổn định &amp; hiệu năng hệ thống</t>
+  </si>
+  <si>
+    <t>Mức độ quan trọng với mục tiêu dự án</t>
+  </si>
+  <si>
+    <t>Giao diện hiển thị và upload ảnh</t>
+  </si>
+  <si>
+    <t>Quản lý dữ liệu và lưu trữ ảnh</t>
+  </si>
+  <si>
+    <t>Mô hình AI nhận dạng</t>
+  </si>
+  <si>
+    <t>Nhận dạng và phân loại đối tượng</t>
   </si>
 </sst>
 </file>
@@ -144,7 +169,133 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -623,7 +774,390 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1"/>
+              <a:t>Tổng</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" baseline="0"/>
+              <a:t> điểm trọng số bởi dự án</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="2000" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$D$2:$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Giao diện hiển thị và upload ảnh</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Quản lý dữ liệu và lưu trữ ảnh</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mô hình AI nhận dạng</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Nhận dạng và phân loại đối tượng</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$7:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>35.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40.450000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36.15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34.299999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3E2E-4763-835D-008D7B75B9BA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1482291456"/>
+        <c:axId val="1482289792"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1482291456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1482289792"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1482289792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1482291456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1168,27 +1702,573 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>9338</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>603370</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>130735</xdr:rowOff>
+      <xdr:rowOff>140977</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>18676</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2476741</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>9338</xdr:rowOff>
+      <xdr:rowOff>19580</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CA1E6CD-5DD4-495E-8E85-3E45EEBB4BBE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFE17F6C-CBC9-4BDE-9E33-EA65D39D1B08}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>15119</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44BA4118-902A-491B-9E32-07C19626C8E5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1210,14 +2290,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9AD20FF1-0E48-492B-AB4D-7877C1E452D4}" name="Table1" displayName="Table1" ref="A2:E12" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9AD20FF1-0E48-492B-AB4D-7877C1E452D4}" name="Table1" displayName="Table1" ref="A2:E12" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A2:E12" xr:uid="{9AD20FF1-0E48-492B-AB4D-7877C1E452D4}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B7ECE57F-3002-4887-94CF-58731BD59B82}" name="STT" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{508C169B-8E43-4C70-8FBA-5369C8E558EF}" name="Tiêu chí" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{7B59BEF9-0B7D-4D0D-A476-E8045CC1526D}" name="WIEGHT" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{19B9B46E-4CB9-4A87-953D-CE3AA1CC55DD}" name="XÂY DỰNG HỆ THỐNG LƯU TRỮ VÀ PHÂN LOẠI ẢNH TRỰC TUYẾN" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{22C54338-5F7E-4FA3-A154-D2CBB98C736C}" name="XÂY DỰNG ỨNG DỤNG NHẬN DẠNG_x000a_ CÁC ĐỐI TƯỢNG TRÊN ẢNH" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{B7ECE57F-3002-4887-94CF-58731BD59B82}" name="STT" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{508C169B-8E43-4C70-8FBA-5369C8E558EF}" name="Tiêu chí" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{7B59BEF9-0B7D-4D0D-A476-E8045CC1526D}" name="WIEGHT" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{19B9B46E-4CB9-4A87-953D-CE3AA1CC55DD}" name="XÂY DỰNG HỆ THỐNG LƯU TRỮ VÀ PHÂN LOẠI ẢNH TRỰC TUYẾN" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{22C54338-5F7E-4FA3-A154-D2CBB98C736C}" name="XÂY DỰNG ỨNG DỤNG NHẬN DẠNG_x000a_ CÁC ĐỐI TƯỢNG TRÊN ẢNH" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A57429A1-C17C-495C-816F-723BD2BB1239}" name="Table13" displayName="Table13" ref="A2:G7" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A2:G7" xr:uid="{A57429A1-C17C-495C-816F-723BD2BB1239}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{D63F7FD7-61D1-4A0A-B0EC-E8CF7553B5BD}" name="STT" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{6E190DB2-7932-4D25-B0CB-ADD478605752}" name="Tiêu chí" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{4AE38DB7-1196-4097-9179-40AA851F3389}" name="WIEGHT" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{36ABC789-84BF-44CD-AE92-E28A8E266284}" name="Giao diện hiển thị và upload ảnh" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{F9E85D54-9404-44EA-904F-9720F47B96CD}" name="Quản lý dữ liệu và lưu trữ ảnh" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{C10B6230-FA90-4A62-B0DB-F38C90B3D729}" name="Mô hình AI nhận dạng" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{FB47355B-2F6A-4059-B8B6-F8ADB800420D}" name="Nhận dạng và phân loại đối tượng" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1522,8 +2618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B60778BF-FA04-4B49-9591-560B6ED9F8CE}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -1743,4 +2839,185 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DFF553B-992D-4E39-9524-ACC5B948F180}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView zoomScale="41" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="45" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="46.7265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="D3" s="1">
+        <v>90</v>
+      </c>
+      <c r="E3" s="1">
+        <v>85</v>
+      </c>
+      <c r="F3" s="1">
+        <v>60</v>
+      </c>
+      <c r="G3" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="D4" s="1">
+        <v>70</v>
+      </c>
+      <c r="E4" s="1">
+        <v>85</v>
+      </c>
+      <c r="F4" s="1">
+        <v>80</v>
+      </c>
+      <c r="G4" s="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>65</v>
+      </c>
+      <c r="E5" s="1">
+        <v>90</v>
+      </c>
+      <c r="F5" s="1">
+        <v>85</v>
+      </c>
+      <c r="G5" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>70</v>
+      </c>
+      <c r="E6" s="1">
+        <v>85</v>
+      </c>
+      <c r="F6" s="1">
+        <v>95</v>
+      </c>
+      <c r="G6" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="4">
+        <f>SUM(C3:C6)</f>
+        <v>0.47000000000000003</v>
+      </c>
+      <c r="D7" s="1">
+        <f>SUMPRODUCT(C3:C6,D3:D6)</f>
+        <v>35.4</v>
+      </c>
+      <c r="E7" s="1">
+        <f>SUMPRODUCT(C3:C6,E3:E6)</f>
+        <v>40.450000000000003</v>
+      </c>
+      <c r="F7" s="1">
+        <f>SUMPRODUCT(C3:C6,F3:F6)</f>
+        <v>36.15</v>
+      </c>
+      <c r="G7" s="1">
+        <f>SUMPRODUCT(C3:C6,G3:G6)</f>
+        <v>34.299999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>